<commit_message>
step definition is completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Task1.xlsx
+++ b/src/test/resources/testData/Task1.xlsx
@@ -26,7 +26,7 @@
     <t>App Name</t>
   </si>
   <si>
-    <t>TekCollect</t>
+    <t>SmartCollect</t>
   </si>
   <si>
     <t>Optometry</t>
@@ -35,13 +35,13 @@
     <t>Revenue Cycle</t>
   </si>
   <si>
-    <t>SmartCollect</t>
-  </si>
-  <si>
     <t>CapitalAccounts</t>
   </si>
   <si>
     <t>Abellaregistration</t>
+  </si>
+  <si>
+    <t>TekCollect</t>
   </si>
 </sst>
 </file>
@@ -76,7 +76,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="lightTrellis">
+      <patternFill patternType="solid">
         <fgColor indexed="46"/>
       </patternFill>
     </fill>

</xml_diff>